<commit_message>
11012017 - implementacao de alteracoes no formulario de configuracao, implementado verificacao de espaco no vinculo de tabela
</commit_message>
<xml_diff>
--- a/_install/TABELA_DADOS_MONITORAMENTO_teste.xlsx
+++ b/_install/TABELA_DADOS_MONITORAMENTO_teste.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\eficazmonitor\_install\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="195" windowWidth="20115" windowHeight="7875"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
   <si>
     <t>IMEI (NºSIM)</t>
   </si>
@@ -128,12 +133,30 @@
   </si>
   <si>
     <t>TABELA DE INFORMAÇÕES SIM 900 (PROJETO MONITORAMENTO) - Teste</t>
+  </si>
+  <si>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>float/10</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t xml:space="preserve">float </t>
+  </si>
+  <si>
+    <t>v1.v2.v3.v4.v5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -340,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,15 +462,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -468,6 +482,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,7 +520,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -532,9 +558,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -567,9 +593,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -602,9 +645,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -781,7 +841,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="O4" sqref="O4:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,36 +852,36 @@
     <col min="9" max="9" width="7.85546875" customWidth="1"/>
     <col min="10" max="10" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" customWidth="1"/>
+    <col min="12" max="14" width="8" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44"/>
+      <c r="T1" s="44"/>
       <c r="U1" s="26"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -891,29 +951,29 @@
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
       <c r="H3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="38" t="s">
+      <c r="I3" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="39"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="41" t="s">
+      <c r="J3" s="46"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
       <c r="O3" s="11" t="s">
         <v>34</v>
       </c>
@@ -956,7 +1016,7 @@
       <c r="G4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="40" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="9" t="s">
@@ -977,7 +1037,7 @@
       <c r="N4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="43" t="s">
+      <c r="O4" s="40" t="s">
         <v>28</v>
       </c>
       <c r="P4" s="17" t="s">
@@ -1019,7 +1079,7 @@
       <c r="G5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="43"/>
+      <c r="H5" s="40"/>
       <c r="I5" s="9" t="s">
         <v>25</v>
       </c>
@@ -1038,7 +1098,7 @@
       <c r="N5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="43"/>
+      <c r="O5" s="40"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
@@ -1068,7 +1128,7 @@
       <c r="G6" s="13">
         <v>127</v>
       </c>
-      <c r="H6" s="44" t="s">
+      <c r="H6" s="41" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="8">
@@ -1089,7 +1149,7 @@
       <c r="N6" s="13">
         <v>127</v>
       </c>
-      <c r="O6" s="44" t="s">
+      <c r="O6" s="41" t="s">
         <v>28</v>
       </c>
       <c r="P6" s="15"/>
@@ -1121,7 +1181,7 @@
       <c r="G7" s="33">
         <v>220</v>
       </c>
-      <c r="H7" s="45"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="31">
         <v>220</v>
       </c>
@@ -1140,7 +1200,7 @@
       <c r="N7" s="33">
         <v>220</v>
       </c>
-      <c r="O7" s="45"/>
+      <c r="O7" s="42"/>
       <c r="P7" s="34"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
@@ -1149,26 +1209,66 @@
       <c r="U7" s="29"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-      <c r="P8" s="36"/>
-      <c r="Q8" s="36"/>
-      <c r="R8" s="36"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="36"/>
+      <c r="A8" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="N8" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="O8" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="P8" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="R8" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="S8" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="T8" s="48" t="s">
+        <v>43</v>
+      </c>
       <c r="U8" s="36"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
20012017 - implementacao de listagem de equipamentos para consulta de relatorios, tela de monitoramento foi implementado medicao de bateria
</commit_message>
<xml_diff>
--- a/_install/TABELA_DADOS_MONITORAMENTO_teste.xlsx
+++ b/_install/TABELA_DADOS_MONITORAMENTO_teste.xlsx
@@ -462,6 +462,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,9 +493,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -860,28 +860,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
       <c r="U1" s="26"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -951,29 +951,29 @@
       <c r="A3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="38" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="45" t="s">
+      <c r="I3" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="38" t="s">
+      <c r="J3" s="47"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
       <c r="O3" s="11" t="s">
         <v>34</v>
       </c>
@@ -1016,7 +1016,7 @@
       <c r="G4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="40" t="s">
+      <c r="H4" s="41" t="s">
         <v>28</v>
       </c>
       <c r="I4" s="9" t="s">
@@ -1037,7 +1037,7 @@
       <c r="N4" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="40" t="s">
+      <c r="O4" s="41" t="s">
         <v>28</v>
       </c>
       <c r="P4" s="17" t="s">
@@ -1079,7 +1079,7 @@
       <c r="G5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="40"/>
+      <c r="H5" s="41"/>
       <c r="I5" s="9" t="s">
         <v>25</v>
       </c>
@@ -1098,7 +1098,7 @@
       <c r="N5" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="40"/>
+      <c r="O5" s="41"/>
       <c r="P5" s="15"/>
       <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
@@ -1128,7 +1128,7 @@
       <c r="G6" s="13">
         <v>127</v>
       </c>
-      <c r="H6" s="41" t="s">
+      <c r="H6" s="42" t="s">
         <v>28</v>
       </c>
       <c r="I6" s="8">
@@ -1149,7 +1149,7 @@
       <c r="N6" s="13">
         <v>127</v>
       </c>
-      <c r="O6" s="41" t="s">
+      <c r="O6" s="42" t="s">
         <v>28</v>
       </c>
       <c r="P6" s="15"/>
@@ -1181,7 +1181,7 @@
       <c r="G7" s="33">
         <v>220</v>
       </c>
-      <c r="H7" s="42"/>
+      <c r="H7" s="43"/>
       <c r="I7" s="31">
         <v>220</v>
       </c>
@@ -1200,7 +1200,7 @@
       <c r="N7" s="33">
         <v>220</v>
       </c>
-      <c r="O7" s="42"/>
+      <c r="O7" s="43"/>
       <c r="P7" s="34"/>
       <c r="Q7" s="34"/>
       <c r="R7" s="34"/>
@@ -1230,7 +1230,7 @@
       <c r="G8" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="H8" s="48" t="s">
+      <c r="H8" s="38" t="s">
         <v>40</v>
       </c>
       <c r="I8" s="37" t="s">
@@ -1251,22 +1251,22 @@
       <c r="N8" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="48" t="s">
+      <c r="O8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="P8" s="48" t="s">
+      <c r="P8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="48" t="s">
+      <c r="Q8" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="48" t="s">
+      <c r="R8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="S8" s="48" t="s">
+      <c r="S8" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="T8" s="48" t="s">
+      <c r="T8" s="38" t="s">
         <v>43</v>
       </c>
       <c r="U8" s="36"/>

</xml_diff>

<commit_message>
10/02/2017 - implementacoes de melhorias na tela de monitoramento
</commit_message>
<xml_diff>
--- a/_install/TABELA_DADOS_MONITORAMENTO_teste.xlsx
+++ b/_install/TABELA_DADOS_MONITORAMENTO_teste.xlsx
@@ -123,9 +123,6 @@
     <t>BAT1 - Tensão</t>
   </si>
   <si>
-    <t>BAT1 - Corrente</t>
-  </si>
-  <si>
     <t>0.0.0.0.0</t>
   </si>
   <si>
@@ -151,6 +148,9 @@
   </si>
   <si>
     <t>v1.v2.v3.v4.v5</t>
+  </si>
+  <si>
+    <t>BAT2 - Tensão</t>
   </si>
 </sst>
 </file>
@@ -841,7 +841,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4:O5"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="45"/>
       <c r="C1" s="45"/>
@@ -975,22 +975,22 @@
       <c r="M3" s="40"/>
       <c r="N3" s="40"/>
       <c r="O3" s="11" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S3" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="U3" s="20"/>
     </row>
@@ -1041,19 +1041,19 @@
         <v>28</v>
       </c>
       <c r="P4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="T4" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U4" s="28"/>
     </row>
@@ -1210,64 +1210,64 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="C8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="I8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="K8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="N8" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="O8" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="H8" s="38" t="s">
+      <c r="P8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="N8" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="O8" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="P8" s="38" t="s">
+      <c r="Q8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="38" t="s">
+      <c r="R8" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="38" t="s">
-        <v>43</v>
-      </c>
       <c r="S8" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="T8" s="38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U8" s="36"/>
     </row>

</xml_diff>